<commit_message>
prog CkBead fix & 47 Kezilabda
</commit_message>
<xml_diff>
--- a/1/.prog/beadando/telepules valamikor maximalis homerseklettel/telepules valamikor maximalis homerseklettel.xlsx
+++ b/1/.prog/beadando/telepules valamikor maximalis homerseklettel/telepules valamikor maximalis homerseklettel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lothiard\OneDrive\Asztali gép\ELTE\repo\elte-cs-bsc\1\.prog\beadando\telepules valamikor maximalis homerseklettel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{160C50C7-65B0-4723-99C0-F3369DEC5705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A714587-7348-401A-8EB5-2563AD8ECB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F2316D82-0603-4B91-BFA5-E2FFCD2491C8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F2316D82-0603-4B91-BFA5-E2FFCD2491C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>maxert</t>
   </si>
@@ -59,9 +59,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>ho[telep, i]</t>
-  </si>
-  <si>
     <t>max</t>
   </si>
   <si>
@@ -74,12 +71,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>telepulesmax(i).2</t>
-  </si>
-  <si>
-    <t>telepulesmax(telep)</t>
-  </si>
-  <si>
     <t>bennevan(sor)</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>T(i)</t>
   </si>
   <si>
-    <t>ho[sor, i] = maxho</t>
-  </si>
-  <si>
     <t>kivalogatas</t>
   </si>
   <si>
@@ -102,6 +90,18 @@
   </si>
   <si>
     <t>bennevan(i)</t>
+  </si>
+  <si>
+    <t>n * m</t>
+  </si>
+  <si>
+    <t>ho[(i - 1) div m + 1, (i - 1) mod m + 1]</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>ho[sor, j] = maxho</t>
   </si>
 </sst>
 </file>
@@ -218,23 +218,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -569,196 +568,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEEE822-EF76-4ED3-A6EF-A707AB8CEE24}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="2"/>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="3" t="s">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>